<commit_message>
Add Molecular weight to dapagliflozin data sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/CompiledDataSet.xlsx
+++ b/inst/extdata/CompiledDataSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DBB84F-0938-4610-BCC3-D0486A73C3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EE5E13-A30D-4543-A19F-E3E852525524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="875" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +618,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF192027"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -962,7 +968,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -984,6 +990,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1342,29 +1349,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="A1:N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1408,7 +1415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1433,6 +1440,9 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
+      <c r="I2" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J2">
         <v>144.01598816912113</v>
       </c>
@@ -1446,7 +1456,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1471,6 +1481,9 @@
       <c r="H3" t="s">
         <v>12</v>
       </c>
+      <c r="I3" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J3" s="1">
         <v>144.67036763174102</v>
       </c>
@@ -1484,7 +1497,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1509,6 +1522,9 @@
       <c r="H4" t="s">
         <v>12</v>
       </c>
+      <c r="I4" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J4" s="1">
         <v>145.3957506816262</v>
       </c>
@@ -1522,7 +1538,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1547,6 +1563,9 @@
       <c r="H5" t="s">
         <v>12</v>
       </c>
+      <c r="I5" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J5">
         <v>146.03262190864493</v>
       </c>
@@ -1560,7 +1579,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1585,6 +1604,9 @@
       <c r="H6" t="s">
         <v>12</v>
       </c>
+      <c r="I6" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J6" s="1">
         <v>146.60101688784701</v>
       </c>
@@ -1598,7 +1620,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1623,6 +1645,9 @@
       <c r="H7" t="s">
         <v>12</v>
       </c>
+      <c r="I7" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J7" s="1">
         <v>147.31270102535808</v>
       </c>
@@ -1636,7 +1661,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1661,6 +1686,9 @@
       <c r="H8" t="s">
         <v>12</v>
       </c>
+      <c r="I8" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J8">
         <v>148.02467818773277</v>
       </c>
@@ -1674,7 +1702,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1699,6 +1727,9 @@
       <c r="H9" t="s">
         <v>12</v>
       </c>
+      <c r="I9" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J9" s="1">
         <v>148.73634401118989</v>
       </c>
@@ -1712,7 +1743,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1737,6 +1768,9 @@
       <c r="H10" t="s">
         <v>12</v>
       </c>
+      <c r="I10" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J10" s="1">
         <v>149.34127552807428</v>
       </c>
@@ -1750,7 +1784,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1775,6 +1809,9 @@
       <c r="H11" t="s">
         <v>12</v>
       </c>
+      <c r="I11" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J11">
         <v>150.03481043809506</v>
       </c>
@@ -1788,7 +1825,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1813,6 +1850,9 @@
       <c r="H12" t="s">
         <v>12</v>
       </c>
+      <c r="I12" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J12" s="1">
         <v>150.67492325266755</v>
       </c>
@@ -1826,7 +1866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1851,6 +1891,9 @@
       <c r="H13" t="s">
         <v>12</v>
       </c>
+      <c r="I13" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J13">
         <v>168.0165559047943</v>
       </c>
@@ -1866,6 +1909,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1877,26 +1921,26 @@
       <selection activeCell="M2" sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" customWidth="1"/>
-    <col min="12" max="12" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.54296875" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.06640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.73046875" customWidth="1"/>
+    <col min="12" max="12" width="23.53125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.53125" customWidth="1"/>
+    <col min="14" max="14" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1946,7 +1990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1993,7 +2037,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2040,7 +2084,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2087,7 +2131,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2134,7 +2178,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2181,7 +2225,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2228,7 +2272,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2275,7 +2319,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2322,7 +2366,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2369,7 +2413,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2416,7 +2460,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2463,7 +2507,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2523,9 +2567,9 @@
       <selection sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2575,7 +2619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2622,7 +2666,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2669,7 +2713,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2716,7 +2760,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2763,7 +2807,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2810,7 +2854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2857,7 +2901,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2904,7 +2948,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2951,7 +2995,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2998,7 +3042,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3045,7 +3089,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3092,7 +3136,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -3152,16 +3196,16 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.36328125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.6328125" style="3"/>
+    <col min="1" max="1" width="12.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.59765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
@@ -3176,7 +3220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3193,7 +3237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -3201,10 +3245,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C8" s="4"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
@@ -3212,10 +3256,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C14" s="4"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -3223,7 +3267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
@@ -3240,7 +3284,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E21" s="3" t="s">
         <v>31</v>
       </c>
@@ -3248,7 +3292,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E22" s="3" t="s">
         <v>36</v>
       </c>
@@ -3256,7 +3300,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
@@ -3264,7 +3308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
@@ -3275,7 +3319,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
@@ -3286,7 +3330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
@@ -3300,7 +3344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C27" s="3" t="s">
         <v>47</v>
       </c>
@@ -3328,9 +3372,9 @@
       <selection sqref="A1:N78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3374,7 +3418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -3385,7 +3429,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -3396,7 +3440,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -3407,7 +3451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -3418,7 +3462,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -3429,7 +3473,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -3440,7 +3484,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -3451,7 +3495,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -3462,7 +3506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -3473,7 +3517,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -3484,7 +3528,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -3495,7 +3539,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -3506,7 +3550,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -3517,7 +3561,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -3528,7 +3572,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -3539,7 +3583,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -3550,7 +3594,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -3561,7 +3605,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -3572,7 +3616,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -3583,7 +3627,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -3594,7 +3638,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -3605,7 +3649,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -3616,7 +3660,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -3627,7 +3671,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -3638,7 +3682,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -3649,7 +3693,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -3663,7 +3707,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -3677,7 +3721,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -3691,7 +3735,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -3705,7 +3749,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -3719,7 +3763,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -3733,7 +3777,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -3747,7 +3791,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -3761,7 +3805,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -3775,7 +3819,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -3789,7 +3833,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -3803,7 +3847,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -3814,7 +3858,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -3825,7 +3869,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -3839,7 +3883,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -3853,7 +3897,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -3867,7 +3911,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -3881,7 +3925,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -3895,7 +3939,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -3909,7 +3953,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -3923,7 +3967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -3937,7 +3981,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -3951,7 +3995,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -3965,7 +4009,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -3979,7 +4023,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -3990,7 +4034,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -4001,7 +4045,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -4015,7 +4059,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -4029,7 +4073,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -4043,7 +4087,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -4057,7 +4101,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -4071,7 +4115,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -4085,7 +4129,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -4099,7 +4143,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -4113,7 +4157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -4127,7 +4171,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -4141,7 +4185,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -4155,7 +4199,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -4169,7 +4213,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -4183,7 +4227,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -4197,7 +4241,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -4211,7 +4255,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -4225,7 +4269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -4239,7 +4283,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -4253,7 +4297,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -4267,7 +4311,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -4281,7 +4325,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -4295,7 +4339,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -4309,7 +4353,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -4323,7 +4367,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -4337,7 +4381,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -4351,7 +4395,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -4378,9 +4422,9 @@
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4437,9 +4481,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4483,7 +4527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -4494,7 +4538,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -4505,7 +4549,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -4516,7 +4560,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -4527,7 +4571,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -4541,7 +4585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -4555,7 +4599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -4569,7 +4613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -4580,7 +4624,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -4591,7 +4635,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -4602,7 +4646,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -4613,7 +4657,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -4624,7 +4668,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -4635,7 +4679,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -4646,7 +4690,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -4657,7 +4701,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -4668,7 +4712,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -4679,7 +4723,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -4690,7 +4734,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -4701,7 +4745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -4712,7 +4756,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -4723,7 +4767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -4734,7 +4778,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -4745,7 +4789,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -4756,7 +4800,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -4767,7 +4811,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -4781,7 +4825,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -4795,7 +4839,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -4809,7 +4853,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -4823,7 +4867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -4837,7 +4881,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -4851,7 +4895,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -4865,7 +4909,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -4879,7 +4923,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -4893,7 +4937,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -4907,7 +4951,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -4921,7 +4965,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -4932,7 +4976,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -4943,7 +4987,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -4957,7 +5001,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -4971,7 +5015,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -4985,7 +5029,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -4999,7 +5043,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -5013,7 +5057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -5027,7 +5071,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -5041,7 +5085,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -5055,7 +5099,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -5069,7 +5113,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -5083,7 +5127,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -5097,7 +5141,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -5108,7 +5152,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -5119,7 +5163,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -5133,7 +5177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -5147,7 +5191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -5161,7 +5205,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -5175,7 +5219,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -5189,7 +5233,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -5203,7 +5247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -5217,7 +5261,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -5231,7 +5275,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -5245,7 +5289,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -5259,7 +5303,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -5273,7 +5317,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -5287,7 +5331,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -5301,7 +5345,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -5315,7 +5359,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -5329,7 +5373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -5343,7 +5387,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -5357,7 +5401,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -5371,7 +5415,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -5385,7 +5429,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -5399,7 +5443,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -5413,7 +5457,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -5427,7 +5471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -5441,7 +5485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -5455,7 +5499,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -5469,7 +5513,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -5496,9 +5540,9 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -5542,7 +5586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -5553,7 +5597,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -5564,7 +5608,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -5575,7 +5619,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -5586,7 +5630,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -5600,7 +5644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -5614,7 +5658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -5628,7 +5672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -5639,7 +5683,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -5650,7 +5694,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -5661,7 +5705,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -5672,7 +5716,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -5683,7 +5727,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -5694,7 +5738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -5705,7 +5749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -5716,7 +5760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -5727,7 +5771,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -5738,7 +5782,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -5749,7 +5793,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -5760,7 +5804,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -5771,7 +5815,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -5782,7 +5826,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -5793,7 +5837,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -5804,7 +5848,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -5815,7 +5859,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -5826,7 +5870,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -5840,7 +5884,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -5854,7 +5898,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -5868,7 +5912,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -5882,7 +5926,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -5896,7 +5940,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -5910,7 +5954,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -5924,7 +5968,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -5938,7 +5982,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -5952,7 +5996,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -5966,7 +6010,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -5980,7 +6024,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -5991,7 +6035,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -6002,7 +6046,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -6016,7 +6060,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -6030,7 +6074,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -6044,7 +6088,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -6058,7 +6102,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -6072,7 +6116,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -6086,7 +6130,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -6100,7 +6144,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -6114,7 +6158,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -6128,7 +6172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -6142,7 +6186,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -6156,7 +6200,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -6167,7 +6211,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -6178,7 +6222,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -6192,7 +6236,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -6206,7 +6250,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -6220,7 +6264,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -6234,7 +6278,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -6248,7 +6292,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -6262,7 +6306,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -6276,7 +6320,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -6290,7 +6334,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -6304,7 +6348,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -6318,7 +6362,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -6332,7 +6376,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -6346,7 +6390,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -6360,7 +6404,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -6374,7 +6418,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -6388,7 +6432,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -6402,7 +6446,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -6416,7 +6460,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -6430,7 +6474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -6444,7 +6488,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -6458,7 +6502,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -6472,7 +6516,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -6486,7 +6530,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -6500,7 +6544,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -6514,7 +6558,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -6528,7 +6572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -6551,13 +6595,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F0443C-748E-4809-AAEE-9F7977E77C74}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -6568,7 +6612,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6585,9 +6629,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6808,26 +6855,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6852,9 +6888,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Molecular weight to dapagliflozin data sheet (#1020)
</commit_message>
<xml_diff>
--- a/inst/extdata/CompiledDataSet.xlsx
+++ b/inst/extdata/CompiledDataSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6DBB84F-0938-4610-BCC3-D0486A73C3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EE5E13-A30D-4543-A19F-E3E852525524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="875" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +618,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF192027"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -962,7 +968,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -984,6 +990,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1342,29 +1349,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="A1:N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1408,7 +1415,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1433,6 +1440,9 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
+      <c r="I2" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J2">
         <v>144.01598816912113</v>
       </c>
@@ -1446,7 +1456,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -1471,6 +1481,9 @@
       <c r="H3" t="s">
         <v>12</v>
       </c>
+      <c r="I3" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J3" s="1">
         <v>144.67036763174102</v>
       </c>
@@ -1484,7 +1497,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1509,6 +1522,9 @@
       <c r="H4" t="s">
         <v>12</v>
       </c>
+      <c r="I4" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J4" s="1">
         <v>145.3957506816262</v>
       </c>
@@ -1522,7 +1538,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1547,6 +1563,9 @@
       <c r="H5" t="s">
         <v>12</v>
       </c>
+      <c r="I5" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J5">
         <v>146.03262190864493</v>
       </c>
@@ -1560,7 +1579,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1585,6 +1604,9 @@
       <c r="H6" t="s">
         <v>12</v>
       </c>
+      <c r="I6" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J6" s="1">
         <v>146.60101688784701</v>
       </c>
@@ -1598,7 +1620,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1623,6 +1645,9 @@
       <c r="H7" t="s">
         <v>12</v>
       </c>
+      <c r="I7" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J7" s="1">
         <v>147.31270102535808</v>
       </c>
@@ -1636,7 +1661,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1661,6 +1686,9 @@
       <c r="H8" t="s">
         <v>12</v>
       </c>
+      <c r="I8" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J8">
         <v>148.02467818773277</v>
       </c>
@@ -1674,7 +1702,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1699,6 +1727,9 @@
       <c r="H9" t="s">
         <v>12</v>
       </c>
+      <c r="I9" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J9" s="1">
         <v>148.73634401118989</v>
       </c>
@@ -1712,7 +1743,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1737,6 +1768,9 @@
       <c r="H10" t="s">
         <v>12</v>
       </c>
+      <c r="I10" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J10" s="1">
         <v>149.34127552807428</v>
       </c>
@@ -1750,7 +1784,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -1775,6 +1809,9 @@
       <c r="H11" t="s">
         <v>12</v>
       </c>
+      <c r="I11" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J11">
         <v>150.03481043809506</v>
       </c>
@@ -1788,7 +1825,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -1813,6 +1850,9 @@
       <c r="H12" t="s">
         <v>12</v>
       </c>
+      <c r="I12" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J12" s="1">
         <v>150.67492325266755</v>
       </c>
@@ -1826,7 +1866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -1851,6 +1891,9 @@
       <c r="H13" t="s">
         <v>12</v>
       </c>
+      <c r="I13" s="9">
+        <v>408.87299999999999</v>
+      </c>
       <c r="J13">
         <v>168.0165559047943</v>
       </c>
@@ -1866,6 +1909,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1877,26 +1921,26 @@
       <selection activeCell="M2" sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" customWidth="1"/>
-    <col min="12" max="12" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.54296875" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.06640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.73046875" customWidth="1"/>
+    <col min="12" max="12" width="23.53125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.53125" customWidth="1"/>
+    <col min="14" max="14" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1946,7 +1990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1993,7 +2037,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2040,7 +2084,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2087,7 +2131,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2134,7 +2178,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2181,7 +2225,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2228,7 +2272,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2275,7 +2319,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2322,7 +2366,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2369,7 +2413,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2416,7 +2460,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2463,7 +2507,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2523,9 +2567,9 @@
       <selection sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2575,7 +2619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -2622,7 +2666,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2669,7 +2713,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2716,7 +2760,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -2763,7 +2807,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -2810,7 +2854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2857,7 +2901,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2904,7 +2948,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2951,7 +2995,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2998,7 +3042,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -3045,7 +3089,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3092,7 +3136,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -3152,16 +3196,16 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.36328125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="11.6328125" style="3"/>
+    <col min="1" max="1" width="12.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="11.59765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C1" s="5" t="s">
         <v>14</v>
       </c>
@@ -3176,7 +3220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
@@ -3193,7 +3237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
@@ -3201,10 +3245,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C8" s="4"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
@@ -3212,10 +3256,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C14" s="4"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -3223,7 +3267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
@@ -3240,7 +3284,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E21" s="3" t="s">
         <v>31</v>
       </c>
@@ -3248,7 +3292,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E22" s="3" t="s">
         <v>36</v>
       </c>
@@ -3256,7 +3300,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
       <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
@@ -3264,7 +3308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
@@ -3275,7 +3319,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
@@ -3286,7 +3330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C26" s="3" t="s">
         <v>43</v>
       </c>
@@ -3300,7 +3344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C27" s="3" t="s">
         <v>47</v>
       </c>
@@ -3328,9 +3372,9 @@
       <selection sqref="A1:N78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3374,7 +3418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -3385,7 +3429,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -3396,7 +3440,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -3407,7 +3451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -3418,7 +3462,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -3429,7 +3473,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -3440,7 +3484,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -3451,7 +3495,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -3462,7 +3506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -3473,7 +3517,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -3484,7 +3528,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -3495,7 +3539,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -3506,7 +3550,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -3517,7 +3561,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -3528,7 +3572,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -3539,7 +3583,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -3550,7 +3594,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -3561,7 +3605,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -3572,7 +3616,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -3583,7 +3627,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -3594,7 +3638,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -3605,7 +3649,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -3616,7 +3660,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -3627,7 +3671,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -3638,7 +3682,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -3649,7 +3693,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -3663,7 +3707,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -3677,7 +3721,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -3691,7 +3735,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -3705,7 +3749,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -3719,7 +3763,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -3733,7 +3777,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -3747,7 +3791,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -3761,7 +3805,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -3775,7 +3819,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -3789,7 +3833,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -3803,7 +3847,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -3814,7 +3858,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -3825,7 +3869,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -3839,7 +3883,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -3853,7 +3897,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -3867,7 +3911,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -3881,7 +3925,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -3895,7 +3939,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -3909,7 +3953,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -3923,7 +3967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -3937,7 +3981,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -3951,7 +3995,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -3965,7 +4009,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -3979,7 +4023,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -3990,7 +4034,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -4001,7 +4045,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -4015,7 +4059,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -4029,7 +4073,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -4043,7 +4087,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -4057,7 +4101,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -4071,7 +4115,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -4085,7 +4129,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -4099,7 +4143,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -4113,7 +4157,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -4127,7 +4171,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -4141,7 +4185,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -4155,7 +4199,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -4169,7 +4213,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -4183,7 +4227,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -4197,7 +4241,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -4211,7 +4255,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -4225,7 +4269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -4239,7 +4283,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -4253,7 +4297,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -4267,7 +4311,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -4281,7 +4325,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -4295,7 +4339,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -4309,7 +4353,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -4323,7 +4367,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -4337,7 +4381,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -4351,7 +4395,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -4378,9 +4422,9 @@
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4437,9 +4481,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4483,7 +4527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -4494,7 +4538,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -4505,7 +4549,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -4516,7 +4560,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -4527,7 +4571,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -4541,7 +4585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -4555,7 +4599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -4569,7 +4613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -4580,7 +4624,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -4591,7 +4635,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -4602,7 +4646,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -4613,7 +4657,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -4624,7 +4668,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -4635,7 +4679,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -4646,7 +4690,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -4657,7 +4701,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -4668,7 +4712,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -4679,7 +4723,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -4690,7 +4734,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -4701,7 +4745,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -4712,7 +4756,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -4723,7 +4767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -4734,7 +4778,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -4745,7 +4789,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -4756,7 +4800,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -4767,7 +4811,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -4781,7 +4825,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -4795,7 +4839,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -4809,7 +4853,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -4823,7 +4867,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -4837,7 +4881,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -4851,7 +4895,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -4865,7 +4909,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -4879,7 +4923,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -4893,7 +4937,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -4907,7 +4951,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -4921,7 +4965,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -4932,7 +4976,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -4943,7 +4987,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -4957,7 +5001,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -4971,7 +5015,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -4985,7 +5029,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -4999,7 +5043,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -5013,7 +5057,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -5027,7 +5071,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -5041,7 +5085,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -5055,7 +5099,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -5069,7 +5113,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -5083,7 +5127,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -5097,7 +5141,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -5108,7 +5152,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -5119,7 +5163,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -5133,7 +5177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -5147,7 +5191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -5161,7 +5205,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -5175,7 +5219,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -5189,7 +5233,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -5203,7 +5247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -5217,7 +5261,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -5231,7 +5275,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -5245,7 +5289,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -5259,7 +5303,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -5273,7 +5317,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -5287,7 +5331,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -5301,7 +5345,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -5315,7 +5359,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -5329,7 +5373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -5343,7 +5387,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -5357,7 +5401,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -5371,7 +5415,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -5385,7 +5429,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -5399,7 +5443,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -5413,7 +5457,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -5427,7 +5471,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -5441,7 +5485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -5455,7 +5499,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -5469,7 +5513,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -5496,9 +5540,9 @@
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -5542,7 +5586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J2">
         <v>0</v>
       </c>
@@ -5553,7 +5597,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J3">
         <v>13.172268907563</v>
       </c>
@@ -5564,7 +5608,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J4">
         <v>29.403361344537799</v>
       </c>
@@ -5575,7 +5619,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J5">
         <v>44.647058823529399</v>
       </c>
@@ -5586,7 +5630,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J6">
         <v>73.079831932773104</v>
       </c>
@@ -5600,7 +5644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J7">
         <v>88.273109243697405</v>
       </c>
@@ -5614,7 +5658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J8">
         <v>105.48319327730999</v>
       </c>
@@ -5628,7 +5672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J9">
         <v>118.66386554621801</v>
       </c>
@@ -5639,7 +5683,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J10">
         <v>149.029411764705</v>
       </c>
@@ -5650,7 +5694,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J11">
         <v>180.35294117647001</v>
       </c>
@@ -5661,7 +5705,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J12">
         <v>210.65966386554601</v>
       </c>
@@ -5672,7 +5716,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J13">
         <v>240.94537815126</v>
       </c>
@@ -5683,7 +5727,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J14">
         <v>0</v>
       </c>
@@ -5694,7 +5738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J15">
         <v>14.218487394957901</v>
       </c>
@@ -5705,7 +5749,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="J16">
         <v>27.403361344537799</v>
       </c>
@@ -5716,7 +5760,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J17">
         <v>43.634453781512597</v>
       </c>
@@ -5727,7 +5771,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J18">
         <v>57.8403361344537</v>
       </c>
@@ -5738,7 +5782,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J19">
         <v>74.067226890756302</v>
       </c>
@@ -5749,7 +5793,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J20">
         <v>89.260504201680604</v>
       </c>
@@ -5760,7 +5804,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J21">
         <v>105.462184873949</v>
       </c>
@@ -5771,7 +5815,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J22">
         <v>119.642857142857</v>
       </c>
@@ -5782,7 +5826,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J23">
         <v>150.004201680672</v>
       </c>
@@ -5793,7 +5837,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J24">
         <v>179.31932773109199</v>
       </c>
@@ -5804,7 +5848,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J25">
         <v>209.62605042016801</v>
       </c>
@@ -5815,7 +5859,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J26">
         <v>240.915966386554</v>
       </c>
@@ -5826,7 +5870,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J27">
         <v>0.967598097502957</v>
       </c>
@@ -5840,7 +5884,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J28">
         <v>16.306480380499401</v>
       </c>
@@ -5854,7 +5898,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J29">
         <v>30.659928656361402</v>
       </c>
@@ -5868,7 +5912,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J30">
         <v>45.026753864447002</v>
       </c>
@@ -5882,7 +5926,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J31">
         <v>61.475921521997499</v>
       </c>
@@ -5896,7 +5940,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J32">
         <v>74.839476813317404</v>
       </c>
@@ -5910,7 +5954,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J33">
         <v>90.303210463733507</v>
       </c>
@@ -5924,7 +5968,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J34">
         <v>105.76248513674101</v>
       </c>
@@ -5938,7 +5982,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J35">
         <v>121.23513674197299</v>
       </c>
@@ -5952,7 +5996,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J36">
         <v>150.133769322235</v>
       </c>
@@ -5966,7 +6010,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J37">
         <v>182.16260404280601</v>
       </c>
@@ -5980,7 +6024,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J38">
         <v>211.09690844233</v>
       </c>
@@ -5991,7 +6035,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J39">
         <v>242.11355529131899</v>
       </c>
@@ -6002,7 +6046,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J40">
         <v>0.967598097502957</v>
       </c>
@@ -6016,7 +6060,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J41">
         <v>16.306480380499401</v>
       </c>
@@ -6030,7 +6074,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J42">
         <v>30.659928656361402</v>
       </c>
@@ -6044,7 +6088,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J43">
         <v>45.026753864447002</v>
       </c>
@@ -6058,7 +6102,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J44">
         <v>61.475921521997499</v>
       </c>
@@ -6072,7 +6116,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J45">
         <v>74.839476813317404</v>
       </c>
@@ -6086,7 +6130,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J46">
         <v>90.303210463733507</v>
       </c>
@@ -6100,7 +6144,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J47">
         <v>105.76248513674101</v>
       </c>
@@ -6114,7 +6158,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J48">
         <v>121.23513674197299</v>
       </c>
@@ -6128,7 +6172,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J49">
         <v>150.133769322235</v>
       </c>
@@ -6142,7 +6186,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J50">
         <v>182.16260404280601</v>
       </c>
@@ -6156,7 +6200,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J51">
         <v>211.09690844233</v>
       </c>
@@ -6167,7 +6211,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J52">
         <v>242.11355529131899</v>
       </c>
@@ -6178,7 +6222,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J53">
         <v>0</v>
       </c>
@@ -6192,7 +6236,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J54">
         <v>14.482758620689699</v>
       </c>
@@ -6206,7 +6250,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J55">
         <v>28.965517241379299</v>
       </c>
@@ -6220,7 +6264,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J56">
         <v>45.517241379310398</v>
       </c>
@@ -6234,7 +6278,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J57">
         <v>58.965517241379402</v>
       </c>
@@ -6248,7 +6292,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J58">
         <v>74.482758620689694</v>
       </c>
@@ -6262,7 +6306,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J59">
         <v>88.965517241379402</v>
       </c>
@@ -6276,7 +6320,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J60">
         <v>104.482758620689</v>
       </c>
@@ -6290,7 +6334,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J61">
         <v>120</v>
       </c>
@@ -6304,7 +6348,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J62">
         <v>150</v>
       </c>
@@ -6318,7 +6362,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J63">
         <v>180</v>
       </c>
@@ -6332,7 +6376,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J64">
         <v>211.03448275861999</v>
       </c>
@@ -6346,7 +6390,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J65">
         <v>238.96551724137899</v>
       </c>
@@ -6360,7 +6404,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J66">
         <v>0</v>
       </c>
@@ -6374,7 +6418,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="67" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J67">
         <v>14.482758620689699</v>
       </c>
@@ -6388,7 +6432,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J68">
         <v>26.8965517241379</v>
       </c>
@@ -6402,7 +6446,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J69">
         <v>44.482758620689701</v>
       </c>
@@ -6416,7 +6460,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J70">
         <v>61.034482758620797</v>
       </c>
@@ -6430,7 +6474,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J71">
         <v>74.482758620689694</v>
       </c>
@@ -6444,7 +6488,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J72">
         <v>90.000000000000099</v>
       </c>
@@ -6458,7 +6502,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J73">
         <v>104.482758620689</v>
       </c>
@@ -6472,7 +6516,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J74">
         <v>118.965517241379</v>
       </c>
@@ -6486,7 +6530,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J75">
         <v>148.96551724137899</v>
       </c>
@@ -6500,7 +6544,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J76">
         <v>180</v>
       </c>
@@ -6514,7 +6558,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J77">
         <v>208.96551724137899</v>
       </c>
@@ -6528,7 +6572,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="10:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="10:14" x14ac:dyDescent="0.45">
       <c r="J78">
         <v>240</v>
       </c>
@@ -6551,13 +6595,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F0443C-748E-4809-AAEE-9F7977E77C74}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -6568,7 +6612,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6585,9 +6629,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6808,26 +6855,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6852,9 +6888,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix failing data set
</commit_message>
<xml_diff>
--- a/inst/extdata/CompiledDataSet.xlsx
+++ b/inst/extdata/CompiledDataSet.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EE5E13-A30D-4543-A19F-E3E852525524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7943DC-73C8-4909-A6C4-C9C4BFA5C772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
-    <sheet name="UnitsFromColumn" sheetId="53" r:id="rId2"/>
-    <sheet name="UnitsFromColumn_secondSheet" sheetId="54" r:id="rId3"/>
-    <sheet name="MetaInfo" sheetId="48" r:id="rId4"/>
-    <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId5"/>
-    <sheet name="WrongSheet" sheetId="50" r:id="rId6"/>
-    <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId7"/>
-    <sheet name="CorrectSheet_negativeError" sheetId="52" r:id="rId8"/>
-    <sheet name="DefaultConfig" sheetId="55" r:id="rId9"/>
+    <sheet name="TestSheet_1_withMW" sheetId="56" r:id="rId2"/>
+    <sheet name="UnitsFromColumn" sheetId="53" r:id="rId3"/>
+    <sheet name="UnitsFromColumn_secondSheet" sheetId="54" r:id="rId4"/>
+    <sheet name="MetaInfo" sheetId="48" r:id="rId5"/>
+    <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId6"/>
+    <sheet name="WrongSheet" sheetId="50" r:id="rId7"/>
+    <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId8"/>
+    <sheet name="CorrectSheet_negativeError" sheetId="52" r:id="rId9"/>
+    <sheet name="DefaultConfig" sheetId="55" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="81">
   <si>
     <t>Time [h]</t>
   </si>
@@ -987,10 +988,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1440,9 +1441,7 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I2" s="8"/>
       <c r="J2">
         <v>144.01598816912113</v>
       </c>
@@ -1481,9 +1480,7 @@
       <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I3" s="8"/>
       <c r="J3" s="1">
         <v>144.67036763174102</v>
       </c>
@@ -1522,9 +1519,7 @@
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I4" s="8"/>
       <c r="J4" s="1">
         <v>145.3957506816262</v>
       </c>
@@ -1563,9 +1558,7 @@
       <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I5" s="8"/>
       <c r="J5">
         <v>146.03262190864493</v>
       </c>
@@ -1604,9 +1597,7 @@
       <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I6" s="8"/>
       <c r="J6" s="1">
         <v>146.60101688784701</v>
       </c>
@@ -1645,9 +1636,7 @@
       <c r="H7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="1">
         <v>147.31270102535808</v>
       </c>
@@ -1686,9 +1675,7 @@
       <c r="H8" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I8" s="8"/>
       <c r="J8">
         <v>148.02467818773277</v>
       </c>
@@ -1727,9 +1714,7 @@
       <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I9" s="8"/>
       <c r="J9" s="1">
         <v>148.73634401118989</v>
       </c>
@@ -1768,9 +1753,7 @@
       <c r="H10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I10" s="8"/>
       <c r="J10" s="1">
         <v>149.34127552807428</v>
       </c>
@@ -1809,9 +1792,7 @@
       <c r="H11" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I11" s="8"/>
       <c r="J11">
         <v>150.03481043809506</v>
       </c>
@@ -1850,9 +1831,7 @@
       <c r="H12" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I12" s="8"/>
       <c r="J12" s="1">
         <v>150.67492325266755</v>
       </c>
@@ -1891,9 +1870,7 @@
       <c r="H13" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I13" s="8"/>
       <c r="J13">
         <v>168.0165559047943</v>
       </c>
@@ -1913,7 +1890,595 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F0443C-748E-4809-AAEE-9F7977E77C74}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D1FEA6-7335-4139-8BB2-84D880AE44C5}">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J2">
+        <v>144.01598816912113</v>
+      </c>
+      <c r="K2">
+        <v>5.5757279200000003</v>
+      </c>
+      <c r="L2">
+        <v>1.238466311</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J3" s="1">
+        <v>144.67036763174102</v>
+      </c>
+      <c r="K3">
+        <v>21.677390540000001</v>
+      </c>
+      <c r="L3">
+        <v>22.807093760000001</v>
+      </c>
+      <c r="M3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J4" s="1">
+        <v>145.3957506816262</v>
+      </c>
+      <c r="K4">
+        <v>37.883090729999999</v>
+      </c>
+      <c r="L4">
+        <v>35.70653325</v>
+      </c>
+      <c r="M4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J5">
+        <v>146.03262190864493</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5">
+        <v>27.86415818</v>
+      </c>
+      <c r="M5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J6" s="1">
+        <v>146.60101688784701</v>
+      </c>
+      <c r="K6">
+        <v>53.471729979999999</v>
+      </c>
+      <c r="L6">
+        <v>24.045102759999999</v>
+      </c>
+      <c r="M6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J7" s="1">
+        <v>147.31270102535808</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7">
+        <v>14.964032720000001</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J8">
+        <v>148.02467818773277</v>
+      </c>
+      <c r="K8">
+        <v>39.235579170000001</v>
+      </c>
+      <c r="L8">
+        <v>11.35236649</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J9" s="1">
+        <v>148.73634401118989</v>
+      </c>
+      <c r="K9">
+        <v>33.66594869</v>
+      </c>
+      <c r="L9">
+        <v>10.010472350000001</v>
+      </c>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J10" s="1">
+        <v>149.34127552807428</v>
+      </c>
+      <c r="K10">
+        <v>27.992890379999999</v>
+      </c>
+      <c r="L10">
+        <v>8.1528109959999995</v>
+      </c>
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J11">
+        <v>150.03481043809506</v>
+      </c>
+      <c r="K11">
+        <v>23.455175430000001</v>
+      </c>
+      <c r="L11">
+        <v>8.5651503859999991</v>
+      </c>
+      <c r="M11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J12" s="1">
+        <v>150.67492325266755</v>
+      </c>
+      <c r="K12">
+        <v>20.258821090000001</v>
+      </c>
+      <c r="L12">
+        <v>8.3592855630000003</v>
+      </c>
+      <c r="M12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J13">
+        <v>168.0165559047943</v>
+      </c>
+      <c r="K13">
+        <v>2.066727336</v>
+      </c>
+      <c r="L13">
+        <v>5.6758783739999998</v>
+      </c>
+      <c r="M13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFD6957-D35F-4523-AFA1-EEDCE7E2C39C}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -2559,7 +3124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4F5E7-B3CC-49CB-8009-201040C9557C}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -3188,7 +3753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DF631D-DF5E-4A3F-BA90-F9B6EDEECD77}">
   <dimension ref="C1:I27"/>
   <sheetViews>
@@ -3212,10 +3777,10 @@
       <c r="D1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
@@ -3364,7 +3929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0E8DDA-F3F4-4710-A6B6-93A80B4A8C1A}">
   <dimension ref="A1:N78"/>
   <sheetViews>
@@ -4414,7 +4979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCB5B98-2408-40BA-99F9-228ECCEE7326}">
   <dimension ref="A1:N1"/>
   <sheetViews>
@@ -4473,7 +5038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C19160-8B30-4C70-A987-7318B15033AF}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
@@ -5532,7 +6097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BDD5F-6183-4F95-9E5B-E5759D0B37BB}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
@@ -6591,50 +7156,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F0443C-748E-4809-AAEE-9F7977E77C74}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6855,15 +7380,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6888,17 +7424,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Unit converter can transform LLOQ columns (#1021)
</commit_message>
<xml_diff>
--- a/inst/extdata/CompiledDataSet.xlsx
+++ b/inst/extdata/CompiledDataSet.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite-R\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EE5E13-A30D-4543-A19F-E3E852525524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7943DC-73C8-4909-A6C4-C9C4BFA5C772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet_1" sheetId="1" r:id="rId1"/>
-    <sheet name="UnitsFromColumn" sheetId="53" r:id="rId2"/>
-    <sheet name="UnitsFromColumn_secondSheet" sheetId="54" r:id="rId3"/>
-    <sheet name="MetaInfo" sheetId="48" r:id="rId4"/>
-    <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId5"/>
-    <sheet name="WrongSheet" sheetId="50" r:id="rId6"/>
-    <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId7"/>
-    <sheet name="CorrectSheet_negativeError" sheetId="52" r:id="rId8"/>
-    <sheet name="DefaultConfig" sheetId="55" r:id="rId9"/>
+    <sheet name="TestSheet_1_withMW" sheetId="56" r:id="rId2"/>
+    <sheet name="UnitsFromColumn" sheetId="53" r:id="rId3"/>
+    <sheet name="UnitsFromColumn_secondSheet" sheetId="54" r:id="rId4"/>
+    <sheet name="MetaInfo" sheetId="48" r:id="rId5"/>
+    <sheet name="Stevens_2012_placebo" sheetId="49" r:id="rId6"/>
+    <sheet name="WrongSheet" sheetId="50" r:id="rId7"/>
+    <sheet name="CorrectSheet_additionalCols" sheetId="51" r:id="rId8"/>
+    <sheet name="CorrectSheet_negativeError" sheetId="52" r:id="rId9"/>
+    <sheet name="DefaultConfig" sheetId="55" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="81">
   <si>
     <t>Time [h]</t>
   </si>
@@ -987,10 +988,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1440,9 +1441,7 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I2" s="8"/>
       <c r="J2">
         <v>144.01598816912113</v>
       </c>
@@ -1481,9 +1480,7 @@
       <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I3" s="8"/>
       <c r="J3" s="1">
         <v>144.67036763174102</v>
       </c>
@@ -1522,9 +1519,7 @@
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I4" s="8"/>
       <c r="J4" s="1">
         <v>145.3957506816262</v>
       </c>
@@ -1563,9 +1558,7 @@
       <c r="H5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I5" s="8"/>
       <c r="J5">
         <v>146.03262190864493</v>
       </c>
@@ -1604,9 +1597,7 @@
       <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I6" s="8"/>
       <c r="J6" s="1">
         <v>146.60101688784701</v>
       </c>
@@ -1645,9 +1636,7 @@
       <c r="H7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="1">
         <v>147.31270102535808</v>
       </c>
@@ -1686,9 +1675,7 @@
       <c r="H8" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I8" s="8"/>
       <c r="J8">
         <v>148.02467818773277</v>
       </c>
@@ -1727,9 +1714,7 @@
       <c r="H9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I9" s="8"/>
       <c r="J9" s="1">
         <v>148.73634401118989</v>
       </c>
@@ -1768,9 +1753,7 @@
       <c r="H10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I10" s="8"/>
       <c r="J10" s="1">
         <v>149.34127552807428</v>
       </c>
@@ -1809,9 +1792,7 @@
       <c r="H11" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I11" s="8"/>
       <c r="J11">
         <v>150.03481043809506</v>
       </c>
@@ -1850,9 +1831,7 @@
       <c r="H12" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I12" s="8"/>
       <c r="J12" s="1">
         <v>150.67492325266755</v>
       </c>
@@ -1891,9 +1870,7 @@
       <c r="H13" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="9">
-        <v>408.87299999999999</v>
-      </c>
+      <c r="I13" s="8"/>
       <c r="J13">
         <v>168.0165559047943</v>
       </c>
@@ -1913,7 +1890,595 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F0443C-748E-4809-AAEE-9F7977E77C74}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D1FEA6-7335-4139-8BB2-84D880AE44C5}">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J2">
+        <v>144.01598816912113</v>
+      </c>
+      <c r="K2">
+        <v>5.5757279200000003</v>
+      </c>
+      <c r="L2">
+        <v>1.238466311</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J3" s="1">
+        <v>144.67036763174102</v>
+      </c>
+      <c r="K3">
+        <v>21.677390540000001</v>
+      </c>
+      <c r="L3">
+        <v>22.807093760000001</v>
+      </c>
+      <c r="M3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J4" s="1">
+        <v>145.3957506816262</v>
+      </c>
+      <c r="K4">
+        <v>37.883090729999999</v>
+      </c>
+      <c r="L4">
+        <v>35.70653325</v>
+      </c>
+      <c r="M4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J5">
+        <v>146.03262190864493</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5">
+        <v>27.86415818</v>
+      </c>
+      <c r="M5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J6" s="1">
+        <v>146.60101688784701</v>
+      </c>
+      <c r="K6">
+        <v>53.471729979999999</v>
+      </c>
+      <c r="L6">
+        <v>24.045102759999999</v>
+      </c>
+      <c r="M6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J7" s="1">
+        <v>147.31270102535808</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7">
+        <v>14.964032720000001</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J8">
+        <v>148.02467818773277</v>
+      </c>
+      <c r="K8">
+        <v>39.235579170000001</v>
+      </c>
+      <c r="L8">
+        <v>11.35236649</v>
+      </c>
+      <c r="M8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J9" s="1">
+        <v>148.73634401118989</v>
+      </c>
+      <c r="K9">
+        <v>33.66594869</v>
+      </c>
+      <c r="L9">
+        <v>10.010472350000001</v>
+      </c>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J10" s="1">
+        <v>149.34127552807428</v>
+      </c>
+      <c r="K10">
+        <v>27.992890379999999</v>
+      </c>
+      <c r="L10">
+        <v>8.1528109959999995</v>
+      </c>
+      <c r="M10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J11">
+        <v>150.03481043809506</v>
+      </c>
+      <c r="K11">
+        <v>23.455175430000001</v>
+      </c>
+      <c r="L11">
+        <v>8.5651503859999991</v>
+      </c>
+      <c r="M11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J12" s="1">
+        <v>150.67492325266755</v>
+      </c>
+      <c r="K12">
+        <v>20.258821090000001</v>
+      </c>
+      <c r="L12">
+        <v>8.3592855630000003</v>
+      </c>
+      <c r="M12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="8">
+        <v>408.87299999999999</v>
+      </c>
+      <c r="J13">
+        <v>168.0165559047943</v>
+      </c>
+      <c r="K13">
+        <v>2.066727336</v>
+      </c>
+      <c r="L13">
+        <v>5.6758783739999998</v>
+      </c>
+      <c r="M13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFD6957-D35F-4523-AFA1-EEDCE7E2C39C}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -2559,7 +3124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4F5E7-B3CC-49CB-8009-201040C9557C}">
   <dimension ref="A1:P13"/>
   <sheetViews>
@@ -3188,7 +3753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DF631D-DF5E-4A3F-BA90-F9B6EDEECD77}">
   <dimension ref="C1:I27"/>
   <sheetViews>
@@ -3212,10 +3777,10 @@
       <c r="D1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="9"/>
       <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
@@ -3364,7 +3929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0E8DDA-F3F4-4710-A6B6-93A80B4A8C1A}">
   <dimension ref="A1:N78"/>
   <sheetViews>
@@ -4414,7 +4979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCB5B98-2408-40BA-99F9-228ECCEE7326}">
   <dimension ref="A1:N1"/>
   <sheetViews>
@@ -4473,7 +5038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C19160-8B30-4C70-A987-7318B15033AF}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
@@ -5532,7 +6097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BDD5F-6183-4F95-9E5B-E5759D0B37BB}">
   <dimension ref="A1:Q78"/>
   <sheetViews>
@@ -6591,50 +7156,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F0443C-748E-4809-AAEE-9F7977E77C74}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6855,15 +7380,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6888,17 +7424,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07F0F837-F7F5-4F1A-B3BF-0AF8EF39D57E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{68DDEE09-40A7-45D2-BB9E-2F87B709C6D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>